<commit_message>
1) Adding new pinouts -- WIP
</commit_message>
<xml_diff>
--- a/Documentation/Datasheets/Rev2 Datasheets/BOM.xlsx
+++ b/Documentation/Datasheets/Rev2 Datasheets/BOM.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="POWER Pinout" sheetId="2" r:id="rId2"/>
+    <sheet name="CORE Pinout" sheetId="4" r:id="rId3"/>
+    <sheet name="COMMS Pinout" sheetId="5" r:id="rId4"/>
+    <sheet name="ANALOG Pinout" sheetId="6" r:id="rId5"/>
+    <sheet name="MEMORY Pinout" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="113">
   <si>
     <t>LSM6DS0</t>
   </si>
@@ -172,13 +176,196 @@
   </si>
   <si>
     <t>2 (Serial Sensors + Memory)</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Vusb</t>
+  </si>
+  <si>
+    <t>Connections</t>
+  </si>
+  <si>
+    <t>Vaux</t>
+  </si>
+  <si>
+    <t>V3.3</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V5.0</t>
+  </si>
+  <si>
+    <t>I3.3in</t>
+  </si>
+  <si>
+    <t>I3.3out</t>
+  </si>
+  <si>
+    <t>IV1in</t>
+  </si>
+  <si>
+    <t>IV1out</t>
+  </si>
+  <si>
+    <t>IV2in</t>
+  </si>
+  <si>
+    <t>Iv2out</t>
+  </si>
+  <si>
+    <t>I5Vin</t>
+  </si>
+  <si>
+    <t>I5Vout</t>
+  </si>
+  <si>
+    <t>V1inSel</t>
+  </si>
+  <si>
+    <t>V2inSel</t>
+  </si>
+  <si>
+    <t>V1En</t>
+  </si>
+  <si>
+    <t>V2En</t>
+  </si>
+  <si>
+    <t>V1adj</t>
+  </si>
+  <si>
+    <t>V2adj</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>(1.8V-3.3V via V1adj)</t>
+  </si>
+  <si>
+    <t>(1.8V-3.3V via V2adj)</t>
+  </si>
+  <si>
+    <t>Enables V1</t>
+  </si>
+  <si>
+    <t>Enables V2</t>
+  </si>
+  <si>
+    <t>V1in from +5V to V2</t>
+  </si>
+  <si>
+    <t>V2in from +5V to V1</t>
+  </si>
+  <si>
+    <t>V1 output voltage adjustment</t>
+  </si>
+  <si>
+    <t>V2 output voltage adjustment</t>
+  </si>
+  <si>
+    <t>POWER</t>
+  </si>
+  <si>
+    <t>COMMS</t>
+  </si>
+  <si>
+    <t>CORE</t>
+  </si>
+  <si>
+    <t>ANALOG</t>
+  </si>
+  <si>
+    <t>(input from CORE)</t>
+  </si>
+  <si>
+    <t>onboard barrel (no output)</t>
+  </si>
+  <si>
+    <t>Either Vusb or Vaux</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>Switches from Vusb to Vaux</t>
+  </si>
+  <si>
+    <t>VauxEn</t>
+  </si>
+  <si>
+    <t>Spare</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>J7(SW)</t>
+  </si>
+  <si>
+    <t>J8(S)</t>
+  </si>
+  <si>
+    <t>J9(SE)</t>
+  </si>
+  <si>
+    <t>J1(NW)V</t>
+  </si>
+  <si>
+    <t>J3(S)V</t>
+  </si>
+  <si>
+    <t>J5(NE)V</t>
+  </si>
+  <si>
+    <t>J4(SE)H</t>
+  </si>
+  <si>
+    <t>J2(SW)H</t>
+  </si>
+  <si>
+    <t>J2(NE)V</t>
+  </si>
+  <si>
+    <t>(NW)</t>
+  </si>
+  <si>
+    <t>(NE)</t>
+  </si>
+  <si>
+    <t>Comms</t>
+  </si>
+  <si>
+    <t>Analog</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>MEMORY</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Core</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,13 +373,63 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -207,8 +444,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,24 +1064,2917 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="H19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="1"/>
+      <c r="H20" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="D22" s="1"/>
+      <c r="F22" s="2"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>12</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>13</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>14</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>15</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>16</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="D22" s="1"/>
+      <c r="F22" s="2"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>12</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>13</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>14</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>15</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>16</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="D22" s="1"/>
+      <c r="F22" s="2"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>12</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>13</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>14</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>15</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>16</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="D22" s="1"/>
+      <c r="F22" s="2"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>12</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>13</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>14</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>15</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>16</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1) Pie in the sky ideas for Rev2 BOM ...
</commit_message>
<xml_diff>
--- a/Documentation/Datasheets/Rev2 Datasheets/BOM.xlsx
+++ b/Documentation/Datasheets/Rev2 Datasheets/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="12960" windowHeight="8700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,13 @@
     <sheet name="COMMS Pinout" sheetId="5" r:id="rId4"/>
     <sheet name="ANALOG Pinout" sheetId="6" r:id="rId5"/>
     <sheet name="MEMORY Pinout" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="108">
   <si>
     <t>LSM6DS0</t>
   </si>
@@ -271,18 +270,6 @@
     <t>V2 output voltage adjustment</t>
   </si>
   <si>
-    <t>POWER</t>
-  </si>
-  <si>
-    <t>COMMS</t>
-  </si>
-  <si>
-    <t>CORE</t>
-  </si>
-  <si>
-    <t>ANALOG</t>
-  </si>
-  <si>
     <t>(input from CORE)</t>
   </si>
   <si>
@@ -350,9 +337,6 @@
   </si>
   <si>
     <t>Memory</t>
-  </si>
-  <si>
-    <t>MEMORY</t>
   </si>
   <si>
     <t>Power</t>
@@ -770,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,16 +1063,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>54</v>
@@ -1099,19 +1083,19 @@
         <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>53</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1131,7 +1115,7 @@
         <v>55</v>
       </c>
       <c r="I3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1151,7 +1135,7 @@
         <v>59</v>
       </c>
       <c r="I4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1239,7 +1223,7 @@
         <v>53</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>67</v>
@@ -1358,7 +1342,7 @@
         <v>69</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>72</v>
@@ -1421,10 +1405,10 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F20" s="1"/>
       <c r="H20" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I20" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1445,10 +1429,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H23" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I23" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1504,22 +1488,22 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
@@ -1533,19 +1517,19 @@
         <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -1718,7 +1702,7 @@
         <v>53</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>53</v>
@@ -1858,7 +1842,7 @@
         <v>68</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>69</v>
@@ -1923,16 +1907,16 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
@@ -1946,19 +1930,19 @@
         <v>52</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -2127,7 +2111,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
@@ -2141,19 +2125,19 @@
         <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -2326,7 +2310,7 @@
         <v>53</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>53</v>
@@ -2466,7 +2450,7 @@
         <v>68</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>69</v>
@@ -2531,16 +2515,16 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
@@ -2554,19 +2538,19 @@
         <v>52</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -2735,7 +2719,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
@@ -2749,19 +2733,19 @@
         <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -2934,7 +2918,7 @@
         <v>53</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>53</v>
@@ -3074,7 +3058,7 @@
         <v>68</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>69</v>
@@ -3139,16 +3123,16 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
@@ -3162,19 +3146,19 @@
         <v>52</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -3335,7 +3319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
@@ -3343,7 +3327,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
@@ -3357,19 +3341,19 @@
         <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -3542,7 +3526,7 @@
         <v>53</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>53</v>
@@ -3682,7 +3666,7 @@
         <v>68</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>69</v>
@@ -3747,16 +3731,16 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
@@ -3770,19 +3754,19 @@
         <v>52</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -3937,44 +3921,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>